<commit_message>
Added fixes to Ppt
</commit_message>
<xml_diff>
--- a/Trials with XYZ controls enabled.xlsx
+++ b/Trials with XYZ controls enabled.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\elwood.campus.nist.gov\735\users\ems9\My Documents\Summer Media\CRPI-UI-Research-Summer-of-2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01B00459-EA7A-4BBF-897B-36C036911283}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECD25C3-2C9F-4442-BCAE-2B3B34257D20}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="12936"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="user_actions_file_2019_08_02_42" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1177" uniqueCount="163">
   <si>
     <t>Timestamp</t>
   </si>
@@ -489,11 +497,32 @@
   <si>
     <t>Z rotation axis control</t>
   </si>
+  <si>
+    <t>Enable or disable main menu button</t>
+  </si>
+  <si>
+    <t>Pathfinding menu</t>
+  </si>
+  <si>
+    <t>Enable joystics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move speed </t>
+  </si>
+  <si>
+    <t>Reset robot position</t>
+  </si>
+  <si>
+    <t>Open/close gripper</t>
+  </si>
+  <si>
+    <t>Change robots</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1157,6 +1186,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-468C-4788-972C-415E19D19CA5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -1232,6 +1266,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-468C-4788-972C-415E19D19CA5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -1789,7 +1828,7 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>Enable or Disable Main Menu Button</c:v>
+                  <c:v>Enable or disable main menu button</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Z axis control</c:v>
@@ -1810,28 +1849,28 @@
                   <c:v>Free-roam control</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>Pathfinding Menu</c:v>
+                  <c:v>Pathfinding menu</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Enable Joystics</c:v>
+                  <c:v>Enable joystics</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Shift mode</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>Move Speed </c:v>
+                  <c:v>Move speed </c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>HOME</c:v>
+                  <c:v>Reset robot position</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>Open/Close Gripper</c:v>
+                  <c:v>Open/close gripper</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Change Robots</c:v>
+                  <c:v>Change robots</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>Open/Close Gripper</c:v>
+                  <c:v>Open/close gripper</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2856,11 +2895,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG621"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL5" sqref="AL5"/>
+    <sheetView tabSelected="1" topLeftCell="AF17" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BH32" sqref="BH32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3035,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="AG2" t="s">
-        <v>28</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -3623,7 +3662,7 @@
         <v>4</v>
       </c>
       <c r="AG9" t="s">
-        <v>35</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
@@ -3707,7 +3746,7 @@
         <v>4</v>
       </c>
       <c r="AG10" t="s">
-        <v>36</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
@@ -3875,7 +3914,7 @@
         <v>8</v>
       </c>
       <c r="AG12" t="s">
-        <v>38</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
@@ -3959,7 +3998,7 @@
         <v>1</v>
       </c>
       <c r="AG13" t="s">
-        <v>39</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -4043,7 +4082,7 @@
         <v>6</v>
       </c>
       <c r="AG14" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
@@ -4130,7 +4169,7 @@
         <v>1</v>
       </c>
       <c r="AG15" t="s">
-        <v>124</v>
+        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
@@ -4214,7 +4253,7 @@
         <v>6</v>
       </c>
       <c r="AG16" t="s">
-        <v>53</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:27" x14ac:dyDescent="0.3">

</xml_diff>